<commit_message>
Refactored some code and Added more testcases to the test data Excel Sheet
</commit_message>
<xml_diff>
--- a/AutomationChallenge/TestDataFiles/testData.xlsx
+++ b/AutomationChallenge/TestDataFiles/testData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2BCAC1-7521-43B6-AEF2-B2E08F54E197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5660667B-CB3C-419F-B72C-FFDB0DDBD5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36" yWindow="1584" windowWidth="22980" windowHeight="10128" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>searchText</t>
   </si>
@@ -57,15 +57,35 @@
   </si>
   <si>
     <t>scrollingMethod</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Souq</t>
+  </si>
+  <si>
+    <t>Booking</t>
+  </si>
+  <si>
+    <t>TripAdvisor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -92,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
@@ -440,34 +461,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -494,7 +516,100 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted failures screenshot from Screenshots folder and updated the Excel sheet with only 1 test senario which is Vodafone
</commit_message>
<xml_diff>
--- a/AutomationChallenge/TestDataFiles/testData.xlsx
+++ b/AutomationChallenge/TestDataFiles/testData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5660667B-CB3C-419F-B72C-FFDB0DDBD5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44517AB5-68B1-40D9-9E44-34F370FB1E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36" yWindow="1584" windowWidth="22980" windowHeight="10128" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="2232" windowWidth="22980" windowHeight="10128" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>searchText</t>
   </si>
@@ -57,18 +57,6 @@
   </si>
   <si>
     <t>scrollingMethod</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>Souq</t>
-  </si>
-  <si>
-    <t>Booking</t>
-  </si>
-  <si>
-    <t>TripAdvisor</t>
   </si>
 </sst>
 </file>
@@ -453,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,98 +504,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>